<commit_message>
fix: Make gui_attributes Mandatory for Spinbox in JSON Schema (DEV-2556) (#478)
* Update project.json

* Update properties.xlsx

* Update excel2json-expected-output.json

* Update properties-only.json

* Update properties-output-expected.json
</commit_message>
<xml_diff>
--- a/testdata/excel2json/excel2json_files/test-name (test_label)/properties.xlsx
+++ b/testdata/excel2json/excel2json_files/test-name (test_label)/properties.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10811"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/noraammann/Documents/Cloned_GitHub/dsp-tools/testdata/excel2json/excel2json_files/test-name (test_label)/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BDFBA30-8D3C-0943-9602-144FD1C52BF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+    <workbookView xWindow="480" yWindow="500" windowWidth="36880" windowHeight="15620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="Tabelle1"/>
+    <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="148">
   <si>
     <t>name</t>
   </si>
@@ -463,8 +469,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -541,44 +546,41 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+  <cellXfs count="8">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -589,10 +591,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -630,71 +632,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Times New Roman" script="Arab"/>
-        <a:font typeface="Times New Roman" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="MoolBoran" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Times New Roman" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Arial" script="Arab"/>
-        <a:font typeface="Arial" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="DaunPenh" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Arial" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -722,7 +724,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -745,11 +747,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -758,13 +760,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -774,7 +776,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -783,7 +785,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -792,7 +794,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -800,10 +802,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot rev="0" lon="0" lat="0"/>
+              <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
-              <a:rot rev="1200000" lon="0" lat="0"/>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -868,40 +870,33 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:S28"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1">
-      <pane state="frozen" activePane="bottomLeft" topLeftCell="A2" ySplit="1" xSplit="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O24" sqref="O24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" style="9" width="29.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="9" width="24.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="9" width="18.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="9" width="14.005" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="9" width="14.005" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="9" width="14.005" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="9" width="14.005" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="9" width="14.005" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="9" width="18.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="9" width="18.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="9" width="18.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="9" width="18.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="9" width="18.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="9" width="10.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="15" max="15" style="9" width="17.005" customWidth="1" bestFit="1"/>
-    <col min="16" max="16" style="9" width="23.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="17" max="17" style="9" width="13.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="18" max="18" style="9" width="37.14785714285715" customWidth="1" bestFit="1"/>
-    <col min="19" max="19" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="29.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="8" width="14" bestFit="1" customWidth="1"/>
+    <col min="9" max="13" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="23.1640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="37.1640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
+    <row r="1" spans="1:19" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -947,1059 +942,842 @@
       <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="4"/>
-      <c r="Q1" s="4"/>
-      <c r="R1" s="4"/>
-      <c r="S1" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
-      <c r="A2" s="5" t="s">
+    </row>
+    <row r="2" spans="1:19" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="5" t="s">
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="H2" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="I2" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="J2" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="K2" s="5" t="s">
+      <c r="K2" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="L2" s="5" t="s">
+      <c r="L2" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="M2" s="5" t="s">
+      <c r="M2" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="N2" s="5" t="s">
+      <c r="N2" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="O2" s="5"/>
-      <c r="P2" s="5" t="s">
+      <c r="O2" s="4"/>
+      <c r="P2" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="Q2" s="4"/>
-      <c r="R2" s="5" t="s">
+      <c r="R2" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="S2" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
-      <c r="A3" s="5" t="s">
+    </row>
+    <row r="3" spans="1:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6" t="s">
+      <c r="B3" s="5"/>
+      <c r="C3" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="5" t="s">
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="H3" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="I3" s="5" t="s">
+      <c r="I3" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="J3" s="5" t="s">
+      <c r="J3" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="K3" s="5" t="s">
+      <c r="K3" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="L3" s="5" t="s">
+      <c r="L3" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="M3" s="5" t="s">
+      <c r="M3" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="N3" s="5" t="s">
+      <c r="N3" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="O3" s="5"/>
-      <c r="P3" s="4"/>
-      <c r="Q3" s="5" t="s">
+      <c r="O3" s="4"/>
+      <c r="Q3" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="R3" s="4"/>
-      <c r="S3" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
-      <c r="A4" s="5" t="s">
+    </row>
+    <row r="4" spans="1:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6" t="s">
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="5" t="s">
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="H4" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="I4" s="5" t="s">
+      <c r="I4" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="J4" s="5" t="s">
+      <c r="J4" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="K4" s="5" t="s">
+      <c r="K4" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="L4" s="5" t="s">
+      <c r="L4" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="M4" s="5" t="s">
+      <c r="M4" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="N4" s="5" t="s">
+      <c r="N4" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="O4" s="5" t="s">
+      <c r="O4" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="P4" s="4"/>
-      <c r="Q4" s="5" t="s">
+      <c r="Q4" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="R4" s="5" t="s">
+      <c r="R4" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="S4" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
-      <c r="A5" s="5" t="s">
+    </row>
+    <row r="5" spans="1:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6" t="s">
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="F5" s="6"/>
-      <c r="G5" s="5" t="s">
+      <c r="F5" s="5"/>
+      <c r="G5" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="H5" s="5" t="s">
+      <c r="H5" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="I5" s="5" t="s">
+      <c r="I5" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="J5" s="5" t="s">
+      <c r="J5" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="K5" s="5" t="s">
+      <c r="K5" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="L5" s="5" t="s">
+      <c r="L5" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="M5" s="5" t="s">
+      <c r="M5" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="N5" s="5" t="s">
+      <c r="N5" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="O5" s="5" t="s">
+      <c r="O5" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="P5" s="4"/>
-      <c r="Q5" s="5" t="s">
+      <c r="Q5" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="R5" s="5" t="s">
+      <c r="R5" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="S5" s="5" t="s">
+      <c r="S5" s="4" t="s">
         <v>26</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
-      <c r="A6" s="5" t="s">
+    <row r="6" spans="1:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6" t="s">
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="G6" s="5" t="s">
+      <c r="G6" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="H6" s="5" t="s">
+      <c r="H6" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="I6" s="5" t="s">
+      <c r="I6" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="J6" s="5" t="s">
+      <c r="J6" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="K6" s="5" t="s">
+      <c r="K6" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="L6" s="5" t="s">
+      <c r="L6" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="M6" s="5" t="s">
+      <c r="M6" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="N6" s="5" t="s">
+      <c r="N6" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="O6" s="5"/>
-      <c r="P6" s="5" t="s">
+      <c r="O6" s="4"/>
+      <c r="P6" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="Q6" s="4"/>
-      <c r="R6" s="4"/>
-      <c r="S6" s="5" t="s">
+      <c r="S6" s="4" t="s">
         <v>54</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
-      <c r="A7" s="5" t="s">
+    <row r="7" spans="1:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6" t="s">
+      <c r="C7" s="5"/>
+      <c r="D7" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6" t="s">
+      <c r="E7" s="5"/>
+      <c r="F7" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="G7" s="5" t="s">
+      <c r="G7" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
-      <c r="J7" s="4"/>
-      <c r="K7" s="4"/>
-      <c r="L7" s="5" t="s">
+      <c r="L7" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="M7" s="5" t="s">
+      <c r="M7" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="N7" s="5" t="s">
+      <c r="N7" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="O7" s="5" t="s">
+      <c r="O7" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="P7" s="4"/>
-      <c r="Q7" s="4"/>
-      <c r="R7" s="4"/>
-      <c r="S7" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
-      <c r="A8" s="5" t="s">
+    </row>
+    <row r="8" spans="1:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6" t="s">
+      <c r="C8" s="5"/>
+      <c r="D8" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6" t="s">
+      <c r="E8" s="5"/>
+      <c r="F8" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6" t="s">
+      <c r="G8" s="5"/>
+      <c r="H8" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="I8" s="6"/>
-      <c r="J8" s="6"/>
-      <c r="K8" s="6"/>
-      <c r="L8" s="5" t="s">
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="M8" s="5" t="s">
+      <c r="M8" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="N8" s="5" t="s">
+      <c r="N8" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="O8" s="5"/>
-      <c r="P8" s="4"/>
-      <c r="Q8" s="5" t="s">
+      <c r="O8" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="Q8" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="R8" s="5" t="s">
+      <c r="R8" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="S8" s="5" t="s">
+      <c r="S8" s="4" t="s">
         <v>54</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
-      <c r="A9" s="5" t="s">
+    <row r="9" spans="1:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6" t="s">
+      <c r="C9" s="5"/>
+      <c r="D9" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="E9" s="4"/>
-      <c r="F9" s="6" t="s">
+      <c r="F9" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="6" t="s">
+      <c r="I9" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="J9" s="4"/>
-      <c r="K9" s="4"/>
-      <c r="L9" s="5" t="s">
+      <c r="L9" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="M9" s="5" t="s">
+      <c r="M9" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="N9" s="5" t="s">
+      <c r="N9" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="O9" s="5"/>
-      <c r="P9" s="4"/>
-      <c r="Q9" s="4"/>
-      <c r="R9" s="4"/>
-      <c r="S9" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
-      <c r="A10" s="5" t="s">
+      <c r="O9" s="4"/>
+    </row>
+    <row r="10" spans="1:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="4"/>
-      <c r="J10" s="4"/>
-      <c r="K10" s="6" t="s">
+      <c r="K10" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="L10" s="5" t="s">
+      <c r="L10" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="M10" s="5" t="s">
+      <c r="M10" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="N10" s="5" t="s">
+      <c r="N10" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="O10" s="7"/>
-      <c r="P10" s="4"/>
-      <c r="Q10" s="4"/>
-      <c r="R10" s="4"/>
-      <c r="S10" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
-      <c r="A11" s="5" t="s">
+      <c r="O10" s="6"/>
+    </row>
+    <row r="11" spans="1:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6" t="s">
+      <c r="C11" s="5"/>
+      <c r="D11" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="E11" s="4"/>
-      <c r="F11" s="6" t="s">
+      <c r="F11" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="G11" s="5" t="s">
+      <c r="G11" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="H11" s="5" t="s">
+      <c r="H11" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="I11" s="5" t="s">
+      <c r="I11" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="J11" s="5" t="s">
+      <c r="J11" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="K11" s="5" t="s">
+      <c r="K11" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="L11" s="5" t="s">
+      <c r="L11" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="M11" s="5" t="s">
+      <c r="M11" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="N11" s="5" t="s">
+      <c r="N11" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="O11" s="5"/>
-      <c r="P11" s="4"/>
-      <c r="Q11" s="4"/>
-      <c r="R11" s="4"/>
-      <c r="S11" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
-      <c r="A12" s="5" t="s">
+      <c r="O11" s="4"/>
+    </row>
+    <row r="12" spans="1:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6" t="s">
+      <c r="C12" s="5"/>
+      <c r="D12" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6" t="s">
+      <c r="E12" s="5"/>
+      <c r="F12" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="G12" s="5" t="s">
+      <c r="G12" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="H12" s="5" t="s">
+      <c r="H12" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="I12" s="5" t="s">
+      <c r="I12" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="J12" s="5" t="s">
+      <c r="J12" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="K12" s="5" t="s">
+      <c r="K12" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="L12" s="5" t="s">
+      <c r="L12" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="M12" s="5" t="s">
+      <c r="M12" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="N12" s="5" t="s">
+      <c r="N12" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="O12" s="5"/>
-      <c r="P12" s="7"/>
-      <c r="Q12" s="4" t="s">
+      <c r="O12" s="4"/>
+      <c r="P12" s="6"/>
+      <c r="Q12" t="s">
         <v>25</v>
       </c>
-      <c r="R12" s="4"/>
-      <c r="S12" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
-      <c r="A13" s="5" t="s">
+    </row>
+    <row r="13" spans="1:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="D13" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="E13" s="6" t="s">
+      <c r="E13" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="F13" s="6" t="s">
+      <c r="F13" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="G13" s="6" t="s">
+      <c r="G13" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="H13" s="6" t="s">
+      <c r="H13" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="I13" s="6" t="s">
+      <c r="I13" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="J13" s="6" t="s">
+      <c r="J13" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="K13" s="5" t="s">
+      <c r="K13" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="L13" s="5" t="s">
+      <c r="L13" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="M13" s="5" t="s">
+      <c r="M13" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="N13" s="5" t="s">
+      <c r="N13" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="O13" s="5" t="s">
+      <c r="O13" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="P13" s="4"/>
-      <c r="Q13" s="4"/>
-      <c r="R13" s="4"/>
-      <c r="S13" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
-      <c r="A14" s="5" t="s">
+    </row>
+    <row r="14" spans="1:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C14" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="6" t="s">
+      <c r="F14" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="G14" s="6" t="s">
+      <c r="G14" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="H14" s="6" t="s">
+      <c r="H14" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="I14" s="4"/>
-      <c r="J14" s="4"/>
-      <c r="K14" s="4"/>
-      <c r="L14" s="5" t="s">
+      <c r="L14" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="M14" s="5" t="s">
+      <c r="M14" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="N14" s="5" t="s">
+      <c r="N14" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="O14" s="5"/>
-      <c r="P14" s="4"/>
-      <c r="Q14" s="4" t="s">
+      <c r="O14" s="4"/>
+      <c r="Q14" t="s">
         <v>98</v>
       </c>
-      <c r="R14" s="4"/>
-      <c r="S14" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
-      <c r="A15" s="5" t="s">
+    </row>
+    <row r="15" spans="1:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="B15" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="C15" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="D15" s="6" t="s">
+      <c r="D15" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="E15" s="4"/>
-      <c r="F15" s="6" t="s">
+      <c r="F15" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="G15" s="6" t="s">
+      <c r="G15" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="H15" s="6" t="s">
+      <c r="H15" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="I15" s="6" t="s">
+      <c r="I15" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="J15" s="4"/>
-      <c r="K15" s="4"/>
-      <c r="L15" s="5" t="s">
+      <c r="L15" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="M15" s="5" t="s">
+      <c r="M15" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="N15" s="6" t="s">
+      <c r="N15" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="O15" s="6" t="s">
+      <c r="O15" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="P15" s="4"/>
-      <c r="Q15" s="4"/>
-      <c r="R15" s="4"/>
-      <c r="S15" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
-      <c r="A16" s="5" t="s">
+    </row>
+    <row r="16" spans="1:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="B16" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="C16" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="D16" s="6" t="s">
+      <c r="D16" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="E16" s="4"/>
-      <c r="F16" s="6" t="s">
+      <c r="F16" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="G16" s="6" t="s">
+      <c r="G16" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="H16" s="6" t="s">
+      <c r="H16" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="I16" s="6" t="s">
+      <c r="I16" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="J16" s="4"/>
-      <c r="K16" s="4"/>
-      <c r="L16" s="5" t="s">
+      <c r="L16" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="M16" s="5" t="s">
+      <c r="M16" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="N16" s="5" t="s">
+      <c r="N16" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="O16" s="5"/>
-      <c r="P16" s="4"/>
-      <c r="Q16" s="4"/>
-      <c r="R16" s="4"/>
-      <c r="S16" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
-      <c r="A17" s="5" t="s">
+      <c r="O16" s="4"/>
+    </row>
+    <row r="17" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="B17" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="C17" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="6" t="s">
+      <c r="G17" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="H17" s="6" t="s">
+      <c r="H17" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="I17" s="4"/>
-      <c r="J17" s="4"/>
-      <c r="K17" s="4"/>
-      <c r="L17" s="5" t="s">
+      <c r="L17" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="M17" s="5" t="s">
+      <c r="M17" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="N17" s="5" t="s">
+      <c r="N17" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="O17" s="7"/>
-      <c r="P17" s="4"/>
-      <c r="Q17" s="4"/>
-      <c r="R17" s="4"/>
-      <c r="S17" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
-      <c r="A18" s="5" t="s">
+      <c r="O17" s="6"/>
+    </row>
+    <row r="18" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="B18" s="6" t="s">
+      <c r="B18" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="C18" s="6" t="s">
+      <c r="C18" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
-      <c r="G18" s="6" t="s">
+      <c r="G18" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="H18" s="6" t="s">
+      <c r="H18" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="I18" s="4"/>
-      <c r="J18" s="4"/>
-      <c r="K18" s="4"/>
-      <c r="L18" s="5" t="s">
+      <c r="L18" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="M18" s="5" t="s">
+      <c r="M18" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="N18" s="5" t="s">
+      <c r="N18" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="O18" s="7"/>
-      <c r="P18" s="4"/>
-      <c r="Q18" s="4"/>
-      <c r="R18" s="4"/>
-      <c r="S18" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
-      <c r="A19" s="5" t="s">
+      <c r="O18" s="6"/>
+    </row>
+    <row r="19" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="B19" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="C19" s="6" t="s">
+      <c r="C19" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
-      <c r="G19" s="6" t="s">
+      <c r="G19" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="H19" s="6" t="s">
+      <c r="H19" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="I19" s="4"/>
-      <c r="J19" s="4"/>
-      <c r="K19" s="4"/>
-      <c r="L19" s="5" t="s">
+      <c r="L19" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="M19" s="5" t="s">
+      <c r="M19" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="N19" s="5" t="s">
+      <c r="N19" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="O19" s="7"/>
-      <c r="P19" s="4"/>
-      <c r="Q19" s="4"/>
-      <c r="R19" s="4"/>
-      <c r="S19" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
-      <c r="A20" s="5" t="s">
+      <c r="O19" s="6"/>
+    </row>
+    <row r="20" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="B20" s="6" t="s">
+      <c r="B20" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="C20" s="6" t="s">
+      <c r="C20" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
-      <c r="G20" s="6" t="s">
+      <c r="G20" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="H20" s="6" t="s">
+      <c r="H20" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="I20" s="4"/>
-      <c r="J20" s="4"/>
-      <c r="K20" s="4"/>
-      <c r="L20" s="5" t="s">
+      <c r="L20" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="M20" s="5" t="s">
+      <c r="M20" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="N20" s="5" t="s">
+      <c r="N20" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="O20" s="4"/>
-      <c r="P20" s="4" t="s">
+      <c r="P20" t="s">
         <v>132</v>
       </c>
-      <c r="Q20" s="4"/>
-      <c r="R20" s="4"/>
-      <c r="S20" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
-      <c r="A21" s="4" t="s">
+    </row>
+    <row r="21" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
         <v>133</v>
       </c>
-      <c r="B21" s="6" t="s">
+      <c r="B21" s="5" t="s">
         <v>134</v>
       </c>
-      <c r="C21" s="6"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
-      <c r="G21" s="4"/>
-      <c r="H21" s="4"/>
-      <c r="I21" s="4"/>
-      <c r="J21" s="4"/>
-      <c r="K21" s="4"/>
-      <c r="L21" s="4" t="s">
+      <c r="C21" s="5"/>
+      <c r="L21" t="s">
         <v>22</v>
       </c>
-      <c r="M21" s="4" t="s">
+      <c r="M21" t="s">
         <v>135</v>
       </c>
-      <c r="N21" s="4" t="s">
+      <c r="N21" t="s">
         <v>24</v>
       </c>
-      <c r="O21" s="8" t="s">
+      <c r="O21" s="7" t="s">
         <v>136</v>
       </c>
-      <c r="P21" s="4"/>
-      <c r="Q21" s="4"/>
-      <c r="R21" s="4"/>
-      <c r="S21" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5">
-      <c r="A22" s="5" t="s">
+    </row>
+    <row r="22" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="B22" s="6" t="s">
+      <c r="B22" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="C22" s="6"/>
-      <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="4"/>
-      <c r="G22" s="5"/>
-      <c r="H22" s="5"/>
-      <c r="I22" s="5"/>
-      <c r="J22" s="5"/>
-      <c r="K22" s="5"/>
-      <c r="L22" s="5" t="s">
+      <c r="C22" s="5"/>
+      <c r="G22" s="4"/>
+      <c r="H22" s="4"/>
+      <c r="I22" s="4"/>
+      <c r="J22" s="4"/>
+      <c r="K22" s="4"/>
+      <c r="L22" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="M22" s="5" t="s">
+      <c r="M22" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="N22" s="5" t="s">
+      <c r="N22" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="O22" s="4"/>
-      <c r="P22" s="4"/>
-      <c r="Q22" s="4"/>
-      <c r="R22" s="4"/>
-      <c r="S22" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5">
-      <c r="A23" s="5" t="s">
+    </row>
+    <row r="23" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="B23" s="5" t="s">
+      <c r="B23" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="C23" s="6"/>
-      <c r="D23" s="4"/>
-      <c r="E23" s="4"/>
-      <c r="F23" s="4"/>
-      <c r="G23" s="4"/>
-      <c r="H23" s="4"/>
-      <c r="I23" s="4"/>
-      <c r="J23" s="4"/>
-      <c r="K23" s="4"/>
-      <c r="L23" s="5" t="s">
+      <c r="C23" s="5"/>
+      <c r="L23" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="M23" s="5" t="s">
+      <c r="M23" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="N23" s="5" t="s">
+      <c r="N23" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="O23" s="4"/>
-      <c r="P23" s="4"/>
-      <c r="Q23" s="4"/>
-      <c r="R23" s="4"/>
-      <c r="S23" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="19.5">
-      <c r="A24" s="5" t="s">
+    </row>
+    <row r="24" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="B24" s="5" t="s">
+      <c r="B24" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="C24" s="6"/>
-      <c r="D24" s="4"/>
-      <c r="E24" s="4"/>
-      <c r="F24" s="4"/>
-      <c r="G24" s="4"/>
-      <c r="H24" s="4"/>
-      <c r="I24" s="4"/>
-      <c r="J24" s="4"/>
-      <c r="K24" s="4"/>
-      <c r="L24" s="5" t="s">
+      <c r="C24" s="5"/>
+      <c r="L24" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="M24" s="5" t="s">
+      <c r="M24" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="N24" s="5" t="s">
+      <c r="N24" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="O24" s="4"/>
-      <c r="P24" s="4"/>
-      <c r="Q24" s="4"/>
-      <c r="R24" s="4"/>
-      <c r="S24" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="19.5">
-      <c r="A25" s="5" t="s">
+    </row>
+    <row r="25" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="B25" s="5" t="s">
+      <c r="B25" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="C25" s="6"/>
-      <c r="D25" s="4"/>
-      <c r="E25" s="4"/>
-      <c r="F25" s="4"/>
-      <c r="G25" s="4"/>
-      <c r="H25" s="4"/>
-      <c r="I25" s="4"/>
-      <c r="J25" s="6" t="s">
+      <c r="C25" s="5"/>
+      <c r="J25" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="K25" s="4"/>
-      <c r="L25" s="5" t="s">
+      <c r="L25" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="M25" s="5" t="s">
+      <c r="M25" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="N25" s="5" t="s">
+      <c r="N25" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="O25" s="4"/>
-      <c r="P25" s="4"/>
-      <c r="Q25" s="4"/>
-      <c r="R25" s="4"/>
-      <c r="S25" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="19.5">
-      <c r="A26" s="5" t="s">
+    </row>
+    <row r="26" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="B26" s="5" t="s">
+      <c r="B26" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="C26" s="6"/>
-      <c r="D26" s="4"/>
-      <c r="E26" s="4"/>
-      <c r="F26" s="4"/>
-      <c r="G26" s="4"/>
-      <c r="H26" s="4"/>
-      <c r="I26" s="6" t="s">
+      <c r="C26" s="5"/>
+      <c r="I26" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="J26" s="4"/>
-      <c r="K26" s="4"/>
-      <c r="L26" s="5" t="s">
+      <c r="L26" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="M26" s="5" t="s">
+      <c r="M26" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="N26" s="5" t="s">
+      <c r="N26" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="O26" s="4"/>
-      <c r="P26" s="4"/>
-      <c r="Q26" s="4"/>
-      <c r="R26" s="4"/>
-      <c r="S26" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="19.5">
-      <c r="A27" s="5" t="s">
+    </row>
+    <row r="27" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B27" s="4"/>
-      <c r="C27" s="5" t="s">
+      <c r="C27" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D27" s="4"/>
-      <c r="E27" s="4"/>
-      <c r="F27" s="4"/>
-      <c r="G27" s="4"/>
-      <c r="H27" s="4"/>
-      <c r="I27" s="4"/>
-      <c r="J27" s="4"/>
-      <c r="K27" s="6" t="s">
+      <c r="K27" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="L27" s="4"/>
-      <c r="M27" s="4"/>
-      <c r="N27" s="4"/>
-      <c r="O27" s="4"/>
-      <c r="P27" s="4"/>
-      <c r="Q27" s="4"/>
-      <c r="R27" s="4"/>
-      <c r="S27" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="19.5">
-      <c r="A28" s="4"/>
-      <c r="B28" s="5" t="s">
+    </row>
+    <row r="28" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B28" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C28" s="4"/>
-      <c r="D28" s="4"/>
-      <c r="E28" s="4"/>
-      <c r="F28" s="4"/>
-      <c r="G28" s="4"/>
-      <c r="H28" s="4"/>
-      <c r="I28" s="4"/>
-      <c r="J28" s="6" t="s">
+      <c r="J28" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="K28" s="4"/>
-      <c r="L28" s="4"/>
-      <c r="M28" s="4"/>
-      <c r="N28" s="4"/>
-      <c r="O28" s="4"/>
-      <c r="P28" s="4"/>
-      <c r="Q28" s="4"/>
-      <c r="R28" s="4"/>
-      <c r="S28" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
de facto resolve merge conflict with PR #478
</commit_message>
<xml_diff>
--- a/testdata/excel2json/excel2json_files/test-name (test_label)/properties.xlsx
+++ b/testdata/excel2json/excel2json_files/test-name (test_label)/properties.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10811"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nussbaum/Desktop/dsp-tools/testdata/excel2json/excel2json_files/test-name (test_label)/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9A45C37-1C3F-CD4B-9ED8-770A7065FFB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+    <workbookView xWindow="480" yWindow="760" windowWidth="29880" windowHeight="12680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="Tabelle1"/>
+    <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="146">
   <si>
     <t>name</t>
   </si>
@@ -457,8 +463,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -529,47 +534,41 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+  <cellXfs count="8">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -580,10 +579,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -621,71 +620,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Times New Roman" script="Arab"/>
-        <a:font typeface="Times New Roman" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="MoolBoran" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Times New Roman" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Arial" script="Arab"/>
-        <a:font typeface="Arial" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="DaunPenh" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Arial" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -713,7 +712,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -736,11 +735,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -749,13 +748,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -765,7 +764,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -774,7 +773,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -783,7 +782,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -791,10 +790,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot rev="0" lon="0" lat="0"/>
+              <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
-              <a:rot rev="1200000" lon="0" lat="0"/>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -859,40 +858,35 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:S28"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1">
-      <pane state="frozen" activePane="bottomLeft" topLeftCell="A2" ySplit="1" xSplit="0"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O14" sqref="O14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" style="9" width="29.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="10" width="24.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="9" width="18.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="9" width="14.005" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="9" width="14.005" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="9" width="14.005" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="9" width="14.005" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="9" width="14.005" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="9" width="18.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="10" width="18.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="9" width="18.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="9" width="18.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="9" width="18.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="9" width="10.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="15" max="15" style="9" width="17.005" customWidth="1" bestFit="1"/>
-    <col min="16" max="16" style="9" width="23.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="17" max="17" style="9" width="13.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="18" max="18" style="9" width="37.14785714285715" customWidth="1" bestFit="1"/>
-    <col min="19" max="19" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="29.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.33203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="8" width="14" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.33203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="11" max="13" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="23.1640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="37.1640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
+    <row r="1" spans="1:19" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -938,1055 +932,838 @@
       <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="4"/>
-      <c r="Q1" s="4"/>
-      <c r="R1" s="4"/>
-      <c r="S1" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
-      <c r="A2" s="5" t="s">
+    </row>
+    <row r="2" spans="1:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="5" t="s">
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="H2" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="I2" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="J2" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="K2" s="5" t="s">
+      <c r="K2" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="L2" s="5" t="s">
+      <c r="L2" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="M2" s="5" t="s">
+      <c r="M2" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="N2" s="5" t="s">
+      <c r="N2" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="O2" s="5"/>
-      <c r="P2" s="5" t="s">
+      <c r="O2" s="4"/>
+      <c r="P2" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="Q2" s="4"/>
-      <c r="R2" s="5" t="s">
+      <c r="R2" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="S2" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
-      <c r="A3" s="5" t="s">
+    </row>
+    <row r="3" spans="1:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6" t="s">
+      <c r="B3" s="5"/>
+      <c r="C3" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="5" t="s">
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="H3" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="I3" s="5" t="s">
+      <c r="I3" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="J3" s="5" t="s">
+      <c r="J3" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="K3" s="5" t="s">
+      <c r="K3" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="L3" s="5" t="s">
+      <c r="L3" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="M3" s="5" t="s">
+      <c r="M3" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="N3" s="5"/>
-      <c r="O3" s="5"/>
-      <c r="P3" s="4"/>
-      <c r="Q3" s="5" t="s">
+      <c r="N3" s="4"/>
+      <c r="O3" s="4"/>
+      <c r="Q3" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="R3" s="4"/>
-      <c r="S3" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
-      <c r="A4" s="5" t="s">
+    </row>
+    <row r="4" spans="1:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6" t="s">
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="5" t="s">
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="H4" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="I4" s="5" t="s">
+      <c r="I4" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="J4" s="5" t="s">
+      <c r="J4" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="K4" s="5" t="s">
+      <c r="K4" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="L4" s="5" t="s">
+      <c r="L4" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="M4" s="5" t="s">
+      <c r="M4" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="N4" s="5" t="s">
+      <c r="N4" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="O4" s="5" t="s">
+      <c r="O4" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="P4" s="4"/>
-      <c r="Q4" s="5" t="s">
+      <c r="Q4" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="R4" s="5" t="s">
+      <c r="R4" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="S4" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
-      <c r="A5" s="5" t="s">
+    </row>
+    <row r="5" spans="1:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6" t="s">
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="F5" s="6"/>
-      <c r="G5" s="5" t="s">
+      <c r="F5" s="5"/>
+      <c r="G5" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="H5" s="5" t="s">
+      <c r="H5" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="I5" s="5" t="s">
+      <c r="I5" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="J5" s="5" t="s">
+      <c r="J5" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="K5" s="5" t="s">
+      <c r="K5" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="L5" s="5" t="s">
+      <c r="L5" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="M5" s="5" t="s">
+      <c r="M5" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="N5" s="5" t="s">
+      <c r="N5" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="O5" s="5" t="s">
+      <c r="O5" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="P5" s="4"/>
-      <c r="Q5" s="5" t="s">
+      <c r="Q5" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="R5" s="5" t="s">
+      <c r="R5" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="S5" s="5" t="s">
+      <c r="S5" s="4" t="s">
         <v>26</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
-      <c r="A6" s="5" t="s">
+    <row r="6" spans="1:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6" t="s">
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="G6" s="5" t="s">
+      <c r="G6" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="H6" s="5" t="s">
+      <c r="H6" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="I6" s="5" t="s">
+      <c r="I6" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="J6" s="5" t="s">
+      <c r="J6" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="K6" s="5" t="s">
+      <c r="K6" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="L6" s="5" t="s">
+      <c r="L6" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="M6" s="5" t="s">
+      <c r="M6" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="N6" s="5" t="s">
+      <c r="N6" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="O6" s="5"/>
-      <c r="P6" s="5" t="s">
+      <c r="O6" s="4"/>
+      <c r="P6" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="Q6" s="4"/>
-      <c r="R6" s="4"/>
-      <c r="S6" s="5" t="s">
+      <c r="S6" s="4" t="s">
         <v>53</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
-      <c r="A7" s="5" t="s">
+    <row r="7" spans="1:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6" t="s">
+      <c r="C7" s="5"/>
+      <c r="D7" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6" t="s">
+      <c r="E7" s="5"/>
+      <c r="F7" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="G7" s="5" t="s">
+      <c r="G7" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
-      <c r="J7" s="7"/>
-      <c r="K7" s="4"/>
-      <c r="L7" s="5" t="s">
+      <c r="L7" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="M7" s="5" t="s">
+      <c r="M7" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="N7" s="5" t="s">
+      <c r="N7" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="O7" s="5" t="s">
+      <c r="O7" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="P7" s="4"/>
-      <c r="Q7" s="4"/>
-      <c r="R7" s="4"/>
-      <c r="S7" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
-      <c r="A8" s="5" t="s">
+    </row>
+    <row r="8" spans="1:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6" t="s">
+      <c r="C8" s="5"/>
+      <c r="D8" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6" t="s">
+      <c r="E8" s="5"/>
+      <c r="F8" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6" t="s">
+      <c r="G8" s="5"/>
+      <c r="H8" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="I8" s="6"/>
-      <c r="J8" s="6"/>
-      <c r="K8" s="6"/>
-      <c r="L8" s="5" t="s">
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="M8" s="5" t="s">
+      <c r="M8" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="N8" s="5" t="s">
+      <c r="N8" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="O8" s="5"/>
-      <c r="P8" s="4"/>
-      <c r="Q8" s="5" t="s">
+      <c r="O8" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q8" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="R8" s="5" t="s">
+      <c r="R8" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="S8" s="5" t="s">
+      <c r="S8" s="4" t="s">
         <v>53</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
-      <c r="A9" s="5" t="s">
+    <row r="9" spans="1:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6" t="s">
+      <c r="C9" s="5"/>
+      <c r="D9" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="E9" s="4"/>
-      <c r="F9" s="6" t="s">
+      <c r="F9" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="6" t="s">
+      <c r="I9" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="J9" s="7"/>
-      <c r="K9" s="4"/>
-      <c r="L9" s="5" t="s">
+      <c r="L9" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="M9" s="5" t="s">
+      <c r="M9" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="N9" s="5" t="s">
+      <c r="N9" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="O9" s="5"/>
-      <c r="P9" s="4"/>
-      <c r="Q9" s="4"/>
-      <c r="R9" s="4"/>
-      <c r="S9" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
-      <c r="A10" s="5" t="s">
+      <c r="O9" s="4"/>
+    </row>
+    <row r="10" spans="1:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="4"/>
-      <c r="J10" s="7"/>
-      <c r="K10" s="6" t="s">
+      <c r="K10" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="L10" s="5" t="s">
+      <c r="L10" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="M10" s="5" t="s">
+      <c r="M10" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="N10" s="5" t="s">
+      <c r="N10" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="O10" s="5"/>
-      <c r="P10" s="4"/>
-      <c r="Q10" s="4"/>
-      <c r="R10" s="4"/>
-      <c r="S10" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
-      <c r="A11" s="5" t="s">
+      <c r="O10" s="4"/>
+    </row>
+    <row r="11" spans="1:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6" t="s">
+      <c r="C11" s="5"/>
+      <c r="D11" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="E11" s="4"/>
-      <c r="F11" s="6" t="s">
+      <c r="F11" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="G11" s="5" t="s">
+      <c r="G11" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="H11" s="5" t="s">
+      <c r="H11" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="I11" s="5" t="s">
+      <c r="I11" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="J11" s="5" t="s">
+      <c r="J11" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="K11" s="5" t="s">
+      <c r="K11" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="L11" s="5" t="s">
+      <c r="L11" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="M11" s="5" t="s">
+      <c r="M11" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="N11" s="5"/>
-      <c r="O11" s="5"/>
-      <c r="P11" s="4"/>
-      <c r="Q11" s="4"/>
-      <c r="R11" s="4"/>
-      <c r="S11" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
-      <c r="A12" s="5" t="s">
+      <c r="N11" s="4"/>
+      <c r="O11" s="4"/>
+    </row>
+    <row r="12" spans="1:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6" t="s">
+      <c r="C12" s="5"/>
+      <c r="D12" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6" t="s">
+      <c r="E12" s="5"/>
+      <c r="F12" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="G12" s="5" t="s">
+      <c r="G12" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="H12" s="5" t="s">
+      <c r="H12" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="I12" s="5" t="s">
+      <c r="I12" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="J12" s="5" t="s">
+      <c r="J12" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="K12" s="5" t="s">
+      <c r="K12" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="L12" s="5" t="s">
+      <c r="L12" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="M12" s="5" t="s">
+      <c r="M12" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="N12" s="5" t="s">
+      <c r="N12" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="O12" s="5"/>
-      <c r="P12" s="5"/>
-      <c r="Q12" s="4" t="s">
+      <c r="O12" s="4"/>
+      <c r="P12" s="4"/>
+      <c r="Q12" t="s">
         <v>25</v>
       </c>
-      <c r="R12" s="4"/>
-      <c r="S12" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
-      <c r="A13" s="5" t="s">
+    </row>
+    <row r="13" spans="1:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="D13" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="E13" s="6" t="s">
+      <c r="E13" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="F13" s="6" t="s">
+      <c r="F13" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="G13" s="6" t="s">
+      <c r="G13" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="H13" s="6" t="s">
+      <c r="H13" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="I13" s="6" t="s">
+      <c r="I13" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="J13" s="6" t="s">
+      <c r="J13" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="K13" s="5" t="s">
+      <c r="K13" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="L13" s="5" t="s">
+      <c r="L13" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="M13" s="5" t="s">
+      <c r="M13" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="N13" s="5" t="s">
+      <c r="N13" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="O13" s="5" t="s">
+      <c r="O13" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="P13" s="4"/>
-      <c r="Q13" s="4"/>
-      <c r="R13" s="4"/>
-      <c r="S13" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
-      <c r="A14" s="5" t="s">
+    </row>
+    <row r="14" spans="1:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C14" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="6" t="s">
+      <c r="F14" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="G14" s="6" t="s">
+      <c r="G14" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="H14" s="6" t="s">
+      <c r="H14" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="I14" s="4"/>
-      <c r="J14" s="7"/>
-      <c r="K14" s="4"/>
-      <c r="L14" s="5" t="s">
+      <c r="L14" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="M14" s="5" t="s">
+      <c r="M14" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="N14" s="5" t="s">
+      <c r="N14" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="O14" s="5"/>
-      <c r="P14" s="4"/>
-      <c r="Q14" s="4" t="s">
+      <c r="O14" s="4"/>
+      <c r="Q14" t="s">
         <v>96</v>
       </c>
-      <c r="R14" s="4"/>
-      <c r="S14" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
-      <c r="A15" s="5" t="s">
+    </row>
+    <row r="15" spans="1:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="B15" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="C15" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="D15" s="6" t="s">
+      <c r="D15" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="E15" s="4"/>
-      <c r="F15" s="6" t="s">
+      <c r="F15" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="G15" s="6" t="s">
+      <c r="G15" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="H15" s="6" t="s">
+      <c r="H15" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="I15" s="6" t="s">
+      <c r="I15" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="J15" s="7"/>
-      <c r="K15" s="4"/>
-      <c r="L15" s="5" t="s">
+      <c r="L15" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="M15" s="5" t="s">
+      <c r="M15" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="N15" s="6" t="s">
+      <c r="N15" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="O15" s="6" t="s">
+      <c r="O15" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="P15" s="4"/>
-      <c r="Q15" s="4"/>
-      <c r="R15" s="4"/>
-      <c r="S15" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
-      <c r="A16" s="5" t="s">
+    </row>
+    <row r="16" spans="1:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="B16" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="C16" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="D16" s="6" t="s">
+      <c r="D16" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="E16" s="4"/>
-      <c r="F16" s="6" t="s">
+      <c r="F16" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="G16" s="6" t="s">
+      <c r="G16" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="H16" s="6" t="s">
+      <c r="H16" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="I16" s="6" t="s">
+      <c r="I16" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="J16" s="7"/>
-      <c r="K16" s="4"/>
-      <c r="L16" s="5" t="s">
+      <c r="L16" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="M16" s="5" t="s">
+      <c r="M16" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="N16" s="5" t="s">
+      <c r="N16" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="O16" s="5"/>
-      <c r="P16" s="4"/>
-      <c r="Q16" s="4"/>
-      <c r="R16" s="4"/>
-      <c r="S16" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
-      <c r="A17" s="5" t="s">
+      <c r="O16" s="4"/>
+    </row>
+    <row r="17" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="B17" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="C17" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="6" t="s">
+      <c r="G17" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="H17" s="6" t="s">
+      <c r="H17" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="I17" s="4"/>
-      <c r="J17" s="7"/>
-      <c r="K17" s="4"/>
-      <c r="L17" s="5" t="s">
+      <c r="L17" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="M17" s="5" t="s">
+      <c r="M17" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="N17" s="5" t="s">
+      <c r="N17" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="O17" s="5"/>
-      <c r="P17" s="4"/>
-      <c r="Q17" s="4"/>
-      <c r="R17" s="4"/>
-      <c r="S17" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
-      <c r="A18" s="5" t="s">
+      <c r="O17" s="4"/>
+    </row>
+    <row r="18" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="B18" s="6" t="s">
+      <c r="B18" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="C18" s="6" t="s">
+      <c r="C18" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
-      <c r="G18" s="6" t="s">
+      <c r="G18" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="H18" s="6" t="s">
+      <c r="H18" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="I18" s="4"/>
-      <c r="J18" s="7"/>
-      <c r="K18" s="4"/>
-      <c r="L18" s="5" t="s">
+      <c r="L18" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="M18" s="5" t="s">
+      <c r="M18" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="N18" s="5" t="s">
+      <c r="N18" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="O18" s="5"/>
-      <c r="P18" s="4"/>
-      <c r="Q18" s="4"/>
-      <c r="R18" s="4"/>
-      <c r="S18" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
-      <c r="A19" s="5" t="s">
+      <c r="O18" s="4"/>
+    </row>
+    <row r="19" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="B19" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="C19" s="6" t="s">
+      <c r="C19" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
-      <c r="G19" s="6" t="s">
+      <c r="G19" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="H19" s="6" t="s">
+      <c r="H19" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="I19" s="4"/>
-      <c r="J19" s="7"/>
-      <c r="K19" s="4"/>
-      <c r="L19" s="5" t="s">
+      <c r="L19" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="M19" s="5" t="s">
+      <c r="M19" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="N19" s="5" t="s">
+      <c r="N19" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="O19" s="5"/>
-      <c r="P19" s="4"/>
-      <c r="Q19" s="4"/>
-      <c r="R19" s="4"/>
-      <c r="S19" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
-      <c r="A20" s="5" t="s">
+      <c r="O19" s="4"/>
+    </row>
+    <row r="20" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="B20" s="6" t="s">
+      <c r="B20" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="C20" s="6" t="s">
+      <c r="C20" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
-      <c r="G20" s="6" t="s">
+      <c r="G20" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="H20" s="6" t="s">
+      <c r="H20" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="I20" s="4"/>
-      <c r="J20" s="7"/>
-      <c r="K20" s="4"/>
-      <c r="L20" s="5" t="s">
+      <c r="L20" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="M20" s="5" t="s">
+      <c r="M20" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="N20" s="5" t="s">
+      <c r="N20" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="O20" s="4"/>
-      <c r="P20" s="4" t="s">
+      <c r="P20" t="s">
         <v>130</v>
       </c>
-      <c r="Q20" s="4"/>
-      <c r="R20" s="4"/>
-      <c r="S20" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
-      <c r="A21" s="4" t="s">
+    </row>
+    <row r="21" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
         <v>131</v>
       </c>
-      <c r="B21" s="6" t="s">
+      <c r="B21" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="C21" s="6"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
-      <c r="G21" s="4"/>
-      <c r="H21" s="4"/>
-      <c r="I21" s="4"/>
-      <c r="J21" s="7"/>
-      <c r="K21" s="4"/>
-      <c r="L21" s="4" t="s">
+      <c r="C21" s="5"/>
+      <c r="L21" t="s">
         <v>22</v>
       </c>
-      <c r="M21" s="4" t="s">
+      <c r="M21" t="s">
         <v>133</v>
       </c>
-      <c r="N21" s="4" t="s">
+      <c r="N21" t="s">
         <v>24</v>
       </c>
-      <c r="O21" s="8" t="s">
+      <c r="O21" s="7" t="s">
         <v>134</v>
       </c>
-      <c r="P21" s="4"/>
-      <c r="Q21" s="4"/>
-      <c r="R21" s="4"/>
-      <c r="S21" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5">
-      <c r="A22" s="5" t="s">
+    </row>
+    <row r="22" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="B22" s="6" t="s">
+      <c r="B22" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="C22" s="6"/>
-      <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="4"/>
-      <c r="G22" s="5"/>
-      <c r="H22" s="5"/>
-      <c r="I22" s="5"/>
-      <c r="J22" s="5"/>
-      <c r="K22" s="5"/>
-      <c r="L22" s="5" t="s">
+      <c r="C22" s="5"/>
+      <c r="G22" s="4"/>
+      <c r="H22" s="4"/>
+      <c r="I22" s="4"/>
+      <c r="J22" s="4"/>
+      <c r="K22" s="4"/>
+      <c r="L22" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="M22" s="5" t="s">
+      <c r="M22" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="N22" s="5" t="s">
+      <c r="N22" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="O22" s="4"/>
-      <c r="P22" s="4"/>
-      <c r="Q22" s="4"/>
-      <c r="R22" s="4"/>
-      <c r="S22" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5">
-      <c r="A23" s="5" t="s">
+    </row>
+    <row r="23" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="B23" s="5" t="s">
+      <c r="B23" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="C23" s="6"/>
-      <c r="D23" s="4"/>
-      <c r="E23" s="4"/>
-      <c r="F23" s="4"/>
-      <c r="G23" s="4"/>
-      <c r="H23" s="4"/>
-      <c r="I23" s="4"/>
-      <c r="J23" s="7"/>
-      <c r="K23" s="4"/>
-      <c r="L23" s="5" t="s">
+      <c r="C23" s="5"/>
+      <c r="L23" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="M23" s="5" t="s">
+      <c r="M23" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="N23" s="5" t="s">
+      <c r="N23" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="O23" s="4"/>
-      <c r="P23" s="4"/>
-      <c r="Q23" s="4"/>
-      <c r="R23" s="4"/>
-      <c r="S23" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="19.5">
-      <c r="A24" s="5" t="s">
+    </row>
+    <row r="24" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="B24" s="5" t="s">
+      <c r="B24" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="C24" s="6"/>
-      <c r="D24" s="4"/>
-      <c r="E24" s="4"/>
-      <c r="F24" s="4"/>
-      <c r="G24" s="4"/>
-      <c r="H24" s="4"/>
-      <c r="I24" s="4"/>
-      <c r="J24" s="7"/>
-      <c r="K24" s="4"/>
-      <c r="L24" s="5" t="s">
+      <c r="C24" s="5"/>
+      <c r="L24" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="M24" s="5" t="s">
+      <c r="M24" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="N24" s="5" t="s">
+      <c r="N24" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="O24" s="4"/>
-      <c r="P24" s="4"/>
-      <c r="Q24" s="4"/>
-      <c r="R24" s="4"/>
-      <c r="S24" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="19.5">
-      <c r="A25" s="5" t="s">
+    </row>
+    <row r="25" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="B25" s="5" t="s">
+      <c r="B25" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="C25" s="6"/>
-      <c r="D25" s="4"/>
-      <c r="E25" s="4"/>
-      <c r="F25" s="4"/>
-      <c r="G25" s="4"/>
-      <c r="H25" s="4"/>
-      <c r="I25" s="4"/>
-      <c r="J25" s="6" t="s">
+      <c r="C25" s="5"/>
+      <c r="J25" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="K25" s="4"/>
-      <c r="L25" s="5" t="s">
+      <c r="L25" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="M25" s="5" t="s">
+      <c r="M25" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="N25" s="5" t="s">
+      <c r="N25" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="O25" s="4"/>
-      <c r="P25" s="4"/>
-      <c r="Q25" s="4"/>
-      <c r="R25" s="4"/>
-      <c r="S25" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="19.5">
-      <c r="A26" s="5" t="s">
+    </row>
+    <row r="26" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="B26" s="5" t="s">
+      <c r="B26" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="C26" s="6"/>
-      <c r="D26" s="4"/>
-      <c r="E26" s="4"/>
-      <c r="F26" s="4"/>
-      <c r="G26" s="4"/>
-      <c r="H26" s="4"/>
-      <c r="I26" s="6" t="s">
+      <c r="C26" s="5"/>
+      <c r="I26" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="J26" s="7"/>
-      <c r="K26" s="4"/>
-      <c r="L26" s="5" t="s">
+      <c r="L26" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="M26" s="5" t="s">
+      <c r="M26" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="N26" s="5" t="s">
+      <c r="N26" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="O26" s="4"/>
-      <c r="P26" s="4"/>
-      <c r="Q26" s="4"/>
-      <c r="R26" s="4"/>
-      <c r="S26" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="19.5">
-      <c r="A27" s="5" t="s">
+    </row>
+    <row r="27" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B27" s="7"/>
-      <c r="C27" s="5" t="s">
+      <c r="C27" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D27" s="4"/>
-      <c r="E27" s="4"/>
-      <c r="F27" s="4"/>
-      <c r="G27" s="4"/>
-      <c r="H27" s="4"/>
-      <c r="I27" s="4"/>
-      <c r="J27" s="7"/>
-      <c r="K27" s="6" t="s">
+      <c r="K27" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="L27" s="4"/>
-      <c r="M27" s="4"/>
-      <c r="N27" s="4"/>
-      <c r="O27" s="4"/>
-      <c r="P27" s="4"/>
-      <c r="Q27" s="4"/>
-      <c r="R27" s="4"/>
-      <c r="S27" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="19.5">
-      <c r="A28" s="4"/>
-      <c r="B28" s="5" t="s">
+    </row>
+    <row r="28" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B28" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C28" s="4"/>
-      <c r="D28" s="4"/>
-      <c r="E28" s="4"/>
-      <c r="F28" s="4"/>
-      <c r="G28" s="4"/>
-      <c r="H28" s="4"/>
-      <c r="I28" s="4"/>
-      <c r="J28" s="6" t="s">
+      <c r="J28" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="K28" s="4"/>
-      <c r="L28" s="4"/>
-      <c r="M28" s="4"/>
-      <c r="N28" s="4"/>
-      <c r="O28" s="4"/>
-      <c r="P28" s="4"/>
-      <c r="Q28" s="4"/>
-      <c r="R28" s="4"/>
-      <c r="S28" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
feat!: add support for video and audio segments, remove isSequenceOf and standalone interval value (DEV-3439) (#933)
</commit_message>
<xml_diff>
--- a/testdata/excel2json/excel2json_files/test-name (test_label)/properties.xlsx
+++ b/testdata/excel2json/excel2json_files/test-name (test_label)/properties.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10414"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/noraammann/Documents/Cloned_GitHub/dsp-tools/testdata/excel2json/excel2json_files/test-name (test_label)/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nussbaum/Desktop/dsp-tools/testdata/excel2json/excel2json_files/test-name (test_label)/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F11C06C-D0B1-1A41-B8C7-8754B0C740B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C87B451-B67A-8B45-B9E0-233654C83063}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="500" windowWidth="36880" windowHeight="15620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="15620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="145">
   <si>
     <t>name</t>
   </si>
@@ -353,24 +353,6 @@
   </si>
   <si>
     <t>TimeStamp</t>
-  </si>
-  <si>
-    <t>hasInterval</t>
-  </si>
-  <si>
-    <t>Time interval</t>
-  </si>
-  <si>
-    <t>Zeitintervall</t>
-  </si>
-  <si>
-    <t>hasSequenceBounds</t>
-  </si>
-  <si>
-    <t>IntervalValue</t>
-  </si>
-  <si>
-    <t>Interval</t>
   </si>
   <si>
     <t>hasBoolean</t>
@@ -883,11 +865,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:T28"/>
+  <dimension ref="A1:T27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A20" sqref="A20"/>
+      <selection pane="bottomLeft" activeCell="A17" sqref="A17:XFD17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -947,7 +929,7 @@
         <v>12</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>13</v>
@@ -1074,7 +1056,7 @@
         <v>43</v>
       </c>
       <c r="N4" s="4" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="O4" s="4" t="s">
         <v>44</v>
@@ -1243,7 +1225,7 @@
         <v>65</v>
       </c>
       <c r="N8" s="4" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="O8" s="4" t="s">
         <v>66</v>
@@ -1577,144 +1559,135 @@
         <v>113</v>
       </c>
       <c r="L17" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="M17" s="4" t="s">
         <v>114</v>
-      </c>
-      <c r="M17" s="4" t="s">
-        <v>115</v>
       </c>
       <c r="N17" s="4"/>
       <c r="O17" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="P17" s="6"/>
     </row>
     <row r="18" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="B18" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="C18" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="C18" s="5" t="s">
-        <v>119</v>
-      </c>
       <c r="G18" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="H18" s="5" t="s">
         <v>118</v>
-      </c>
-      <c r="H18" s="5" t="s">
-        <v>119</v>
       </c>
       <c r="L18" s="4" t="s">
         <v>42</v>
       </c>
       <c r="M18" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="N18" s="4"/>
       <c r="O18" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="P18" s="6"/>
     </row>
     <row r="19" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="B19" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="C19" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="C19" s="5" t="s">
+      <c r="G19" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="H19" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="L19" s="4" t="s">
         <v>124</v>
-      </c>
-      <c r="G19" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="H19" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="L19" s="4" t="s">
-        <v>42</v>
       </c>
       <c r="M19" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="N19" s="4"/>
+      <c r="N19" s="4" t="s">
+        <v>144</v>
+      </c>
       <c r="O19" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q19" t="s">
         <v>126</v>
       </c>
-      <c r="P19" s="6"/>
     </row>
     <row r="20" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="4" t="s">
+      <c r="A20" t="s">
         <v>127</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="C20" s="5" t="s">
+      <c r="C20" s="5"/>
+      <c r="L20" t="s">
+        <v>22</v>
+      </c>
+      <c r="M20" t="s">
         <v>129</v>
       </c>
-      <c r="G20" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="H20" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="L20" s="4" t="s">
+      <c r="O20" t="s">
+        <v>24</v>
+      </c>
+      <c r="P20" s="7" t="s">
         <v>130</v>
       </c>
-      <c r="M20" s="4" t="s">
+    </row>
+    <row r="21" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="N20" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="O20" s="4" t="s">
+      <c r="B21" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="C21" s="5"/>
+      <c r="G21" s="4"/>
+      <c r="H21" s="4"/>
+      <c r="I21" s="4"/>
+      <c r="J21" s="4"/>
+      <c r="K21" s="4"/>
+      <c r="L21" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="M21" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="N21" s="4"/>
+      <c r="O21" s="4" t="s">
         <v>24</v>
-      </c>
-      <c r="Q20" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="21" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>133</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>134</v>
-      </c>
-      <c r="C21" s="5"/>
-      <c r="L21" t="s">
-        <v>22</v>
-      </c>
-      <c r="M21" t="s">
-        <v>135</v>
-      </c>
-      <c r="O21" t="s">
-        <v>24</v>
-      </c>
-      <c r="P21" s="7" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="22" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
-        <v>137</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>138</v>
+        <v>134</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>134</v>
       </c>
       <c r="C22" s="5"/>
-      <c r="G22" s="4"/>
-      <c r="H22" s="4"/>
-      <c r="I22" s="4"/>
-      <c r="J22" s="4"/>
-      <c r="K22" s="4"/>
       <c r="L22" s="4" t="s">
         <v>22</v>
       </c>
       <c r="M22" s="4" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="N22" s="4"/>
       <c r="O22" s="4" t="s">
@@ -1723,17 +1696,17 @@
     </row>
     <row r="23" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C23" s="5"/>
       <c r="L23" s="4" t="s">
         <v>22</v>
       </c>
       <c r="M23" s="4" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="N23" s="4"/>
       <c r="O23" s="4" t="s">
@@ -1742,17 +1715,20 @@
     </row>
     <row r="24" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="C24" s="5"/>
+      <c r="J24" s="5" t="s">
+        <v>26</v>
+      </c>
       <c r="L24" s="4" t="s">
         <v>22</v>
       </c>
       <c r="M24" s="4" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="N24" s="4"/>
       <c r="O24" s="4" t="s">
@@ -1761,20 +1737,20 @@
     </row>
     <row r="25" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="C25" s="5"/>
-      <c r="J25" s="5" t="s">
+      <c r="I25" s="5" t="s">
         <v>26</v>
       </c>
       <c r="L25" s="4" t="s">
         <v>22</v>
       </c>
       <c r="M25" s="4" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="N25" s="4"/>
       <c r="O25" s="4" t="s">
@@ -1783,42 +1759,20 @@
     </row>
     <row r="26" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
-        <v>146</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>146</v>
-      </c>
-      <c r="C26" s="5"/>
-      <c r="I26" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="L26" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="M26" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="N26" s="4"/>
-      <c r="O26" s="4" t="s">
-        <v>24</v>
+      <c r="C26" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="K26" s="5" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="27" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="4" t="s">
+      <c r="B27" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C27" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="K27" s="5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="28" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B28" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="J28" s="5" t="s">
+      <c r="J27" s="5" t="s">
         <v>26</v>
       </c>
     </row>

</xml_diff>

<commit_message>
write integration tests, draft implementation
</commit_message>
<xml_diff>
--- a/testdata/excel2json/excel2json_files/test-name (test_label)/properties.xlsx
+++ b/testdata/excel2json/excel2json_files/test-name (test_label)/properties.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10727"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nussbaum/Desktop/dsp-tools/testdata/excel2json/excel2json_files/test-name (test_label)/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nussbaum/Desktop/Cloned_GitHub_repos/dsp-tools/testdata/excel2json/excel2json_files/test-name (test_label)/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C87B451-B67A-8B45-B9E0-233654C83063}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1C59DCD-69A6-8943-8622-028BE902F29E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="15620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="147">
   <si>
     <t>name</t>
   </si>
@@ -455,6 +455,12 @@
   </si>
   <si>
     <t>:Image</t>
+  </si>
+  <si>
+    <t>default_permissions_overrule</t>
+  </si>
+  <si>
+    <t>private</t>
   </si>
 </sst>
 </file>
@@ -537,7 +543,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -559,6 +565,12 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -867,9 +879,9 @@
   </sheetPr>
   <dimension ref="A1:T27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A17" sqref="A17:XFD17"/>
+      <selection pane="bottomLeft" activeCell="Q4" sqref="Q4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -937,6 +949,9 @@
       <c r="P1" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="Q1" s="8" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="2" spans="1:20" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
@@ -1019,6 +1034,9 @@
         <v>35</v>
       </c>
       <c r="P3" s="4"/>
+      <c r="Q3" s="9" t="s">
+        <v>146</v>
+      </c>
       <c r="R3" s="4" t="s">
         <v>26</v>
       </c>

</xml_diff>